<commit_message>
updated ecr mapping, profiles and bindings, added introductory text
</commit_message>
<xml_diff>
--- a/docs/ecr.xlsx
+++ b/docs/ecr.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6896" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6896" uniqueCount="481">
   <si>
     <t>Path</t>
   </si>
@@ -505,7 +505,7 @@
     <t>Composition.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter}
+    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/ecr-encounter}
 </t>
   </si>
   <si>
@@ -947,7 +947,7 @@
     <t>Composition.section</t>
   </si>
   <si>
-    <t>eicr-section-slices</t>
+    <t>ecr-section-slices</t>
   </si>
   <si>
     <t>Composition is broken into sections</t>
@@ -1150,19 +1150,13 @@
     <t>.component.section</t>
   </si>
   <si>
-    <t>eicr-slice2</t>
+    <t>ecr-slice2</t>
   </si>
   <si>
     <t>History of Present Illness Section</t>
   </si>
   <si>
     <t>3284-97</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="History of Present Illiness"/&gt;</t>
-  </si>
-  <si>
-    <t>81-7851</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -1178,19 +1172,16 @@
     <t>81-15477</t>
   </si>
   <si>
-    <t>eicr-slice3</t>
+    <t>81-7851</t>
+  </si>
+  <si>
+    <t>ecr-slice3</t>
   </si>
   <si>
     <t>Reason for Visit Section</t>
   </si>
   <si>
     <t>3284-98</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Reason for Visit"/&gt;</t>
-  </si>
-  <si>
-    <t>81-7839</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -1216,19 +1207,16 @@
     <t>81-15429</t>
   </si>
   <si>
-    <t>eicr-slice4</t>
+    <t>81-7839</t>
+  </si>
+  <si>
+    <t>ecr-slice4</t>
   </si>
   <si>
     <t>Social History Section</t>
   </si>
   <si>
     <t>3284-87</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Social History"/&gt;</t>
-  </si>
-  <si>
-    <t>1198- 7938</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -1244,14 +1232,11 @@
     <t>1198-14819</t>
   </si>
   <si>
-    <t>1198- 8708</t>
-  </si>
-  <si>
     <t xml:space="preserve">value:profile}
 </t>
   </si>
   <si>
-    <t>eicr-sh-slices</t>
+    <t>ecr-sh-slices</t>
   </si>
   <si>
     <t xml:space="preserve">Reference {http://hl7.org/fhir/StructureDefinition/Observation}
@@ -1261,10 +1246,10 @@
     <t>todo</t>
   </si>
   <si>
-    <t>eicr-sh-slice1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/eicr-travelhistory}
+    <t>ecr-sh-slice1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/ecr-travelhistory}
 </t>
   </si>
   <si>
@@ -1274,10 +1259,10 @@
 &lt;/valueReference&gt;</t>
   </si>
   <si>
-    <t>eicr-sh-slice2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/eicr-pregnancystatus}
+    <t>ecr-sh-slice2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/ecr-pregnancystatus}
 </t>
   </si>
   <si>
@@ -1287,10 +1272,10 @@
 &lt;/valueReference&gt;</t>
   </si>
   <si>
-    <t>eicr-sh-slice3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/eicr-occupationhistory}
+    <t>ecr-sh-slice3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/ecr-occupationhistory}
 </t>
   </si>
   <si>
@@ -1300,19 +1285,13 @@
 &lt;/valueReference&gt;</t>
   </si>
   <si>
-    <t>eicr-slice5</t>
+    <t>ecr-slice5</t>
   </si>
   <si>
     <t>Problems Section</t>
   </si>
   <si>
     <t>3284-99</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Problems"/&gt;</t>
-  </si>
-  <si>
-    <t>1198- 9181</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -1328,7 +1307,7 @@
     <t>1198-15409</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition}
+    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/ecr-condition}
 </t>
   </si>
   <si>
@@ -1461,19 +1440,13 @@
     <t>Reference.display</t>
   </si>
   <si>
-    <t>eicr-slice6</t>
+    <t>ecr-slice6</t>
   </si>
   <si>
     <t>Medications Administered Section</t>
   </si>
   <si>
     <t>3284-88</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Medications Administered"/&gt;</t>
-  </si>
-  <si>
-    <t>1098-8154</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -1505,19 +1478,13 @@
     <t>1098-8156</t>
   </si>
   <si>
-    <t>eicr-slice7</t>
+    <t>ecr-slice7</t>
   </si>
   <si>
     <t>Results Section</t>
   </si>
   <si>
     <t>3284-89</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Results"/&gt;</t>
-  </si>
-  <si>
-    <t>1198-8892</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -1533,17 +1500,14 @@
     <t>1198-15433</t>
   </si>
   <si>
-    <t>1198-7111</t>
-  </si>
-  <si>
     <t xml:space="preserve">value:type}
 </t>
   </si>
   <si>
-    <t>eicr-res-slices</t>
-  </si>
-  <si>
-    <t>eicr-res-slice1</t>
+    <t>ecr-res-slices</t>
+  </si>
+  <si>
+    <t>ecr-res-slice1</t>
   </si>
   <si>
     <t xml:space="preserve">Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport}
@@ -1562,7 +1526,7 @@
     <t>trigger2</t>
   </si>
   <si>
-    <t>eicr-res-slice2</t>
+    <t>ecr-res-slice2</t>
   </si>
   <si>
     <t xml:space="preserve">Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-observationresults}
@@ -1578,13 +1542,10 @@
     <t>trigger3</t>
   </si>
   <si>
-    <t>eicr-slice8</t>
+    <t>ecr-slice8</t>
   </si>
   <si>
     <t>Lab Order Section</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Lab Orders"/&gt;</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -1597,7 +1558,7 @@
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {http://hl7.org/fhir/StructureDefinition/ProcedureRequest}
+    <t xml:space="preserve">Reference {http://fhir.hl7.org/us/ecr/StructureDefinition/ecr-procedurerequest}
 </t>
   </si>
   <si>
@@ -1610,19 +1571,13 @@
     <t>trigger4</t>
   </si>
   <si>
-    <t>eicr-slice9</t>
+    <t>ecr-slice9</t>
   </si>
   <si>
     <t>Immunizations Section</t>
   </si>
   <si>
     <t>3284-148</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Immunizations"/&gt;</t>
-  </si>
-  <si>
-    <t>1198-9017</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -1636,9 +1591,6 @@
   </si>
   <si>
     <t>1198-15369</t>
-  </si>
-  <si>
-    <t>1198-9018</t>
   </si>
   <si>
     <t xml:space="preserve">Reference {http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization}
@@ -1810,7 +1762,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="48.2421875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="18.98046875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="18.3828125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="40.90625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
@@ -8197,7 +8149,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
         <v>310</v>
       </c>
@@ -8207,13 +8159,13 @@
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F58" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>40</v>
@@ -8241,13 +8193,13 @@
       </c>
       <c r="P58" s="2"/>
       <c r="Q58" t="s" s="2">
-        <v>368</v>
+        <v>40</v>
       </c>
       <c r="R58" t="s" s="2">
         <v>40</v>
       </c>
       <c r="S58" t="s" s="2">
-        <v>368</v>
+        <v>40</v>
       </c>
       <c r="T58" t="s" s="2">
         <v>40</v>
@@ -8298,7 +8250,7 @@
         <v>40</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>369</v>
+        <v>40</v>
       </c>
       <c r="AK58" t="s" s="2">
         <v>190</v>
@@ -8357,10 +8309,10 @@
         <v>40</v>
       </c>
       <c r="R59" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="S59" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="T59" t="s" s="2">
         <v>40</v>
@@ -8411,7 +8363,7 @@
         <v>40</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>135</v>
@@ -8522,7 +8474,7 @@
         <v>40</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>328</v>
@@ -9100,7 +9052,7 @@
         <v>298</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C66" t="s" s="2">
         <v>40</v>
@@ -9125,7 +9077,7 @@
         <v>200</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L66" t="s" s="2">
         <v>301</v>
@@ -9194,7 +9146,7 @@
         <v>304</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AK66" t="s" s="2">
         <v>305</v>
@@ -9537,7 +9489,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
         <v>310</v>
       </c>
@@ -9547,13 +9499,13 @@
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F70" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G70" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H70" t="s" s="2">
         <v>40</v>
@@ -9581,13 +9533,13 @@
       </c>
       <c r="P70" s="2"/>
       <c r="Q70" t="s" s="2">
-        <v>375</v>
+        <v>40</v>
       </c>
       <c r="R70" t="s" s="2">
         <v>40</v>
       </c>
       <c r="S70" t="s" s="2">
-        <v>375</v>
+        <v>40</v>
       </c>
       <c r="T70" t="s" s="2">
         <v>40</v>
@@ -9638,7 +9590,7 @@
         <v>40</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>376</v>
+        <v>40</v>
       </c>
       <c r="AK70" t="s" s="2">
         <v>190</v>
@@ -9697,10 +9649,10 @@
         <v>40</v>
       </c>
       <c r="R71" t="s" s="2">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="S71" t="s" s="2">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="T71" t="s" s="2">
         <v>40</v>
@@ -9751,7 +9703,7 @@
         <v>40</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="AK71" t="s" s="2">
         <v>135</v>
@@ -9862,7 +9814,7 @@
         <v>40</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AK72" t="s" s="2">
         <v>328</v>
@@ -10440,7 +10392,7 @@
         <v>298</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C78" t="s" s="2">
         <v>40</v>
@@ -10465,7 +10417,7 @@
         <v>200</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L78" t="s" s="2">
         <v>301</v>
@@ -10534,7 +10486,7 @@
         <v>304</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AK78" t="s" s="2">
         <v>305</v>
@@ -10877,7 +10829,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
         <v>310</v>
       </c>
@@ -10887,13 +10839,13 @@
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F82" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G82" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H82" t="s" s="2">
         <v>40</v>
@@ -10921,13 +10873,13 @@
       </c>
       <c r="P82" s="2"/>
       <c r="Q82" t="s" s="2">
-        <v>383</v>
+        <v>40</v>
       </c>
       <c r="R82" t="s" s="2">
         <v>40</v>
       </c>
       <c r="S82" t="s" s="2">
-        <v>383</v>
+        <v>40</v>
       </c>
       <c r="T82" t="s" s="2">
         <v>40</v>
@@ -10978,7 +10930,7 @@
         <v>40</v>
       </c>
       <c r="AJ82" t="s" s="2">
-        <v>384</v>
+        <v>40</v>
       </c>
       <c r="AK82" t="s" s="2">
         <v>190</v>
@@ -11037,10 +10989,10 @@
         <v>40</v>
       </c>
       <c r="R83" t="s" s="2">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="S83" t="s" s="2">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="T83" t="s" s="2">
         <v>40</v>
@@ -11091,7 +11043,7 @@
         <v>40</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="AK83" t="s" s="2">
         <v>135</v>
@@ -11103,7 +11055,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
         <v>323</v>
       </c>
@@ -11113,13 +11065,13 @@
       </c>
       <c r="D84" s="2"/>
       <c r="E84" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F84" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G84" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H84" t="s" s="2">
         <v>40</v>
@@ -11202,7 +11154,7 @@
         <v>40</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>387</v>
+        <v>40</v>
       </c>
       <c r="AK84" t="s" s="2">
         <v>328</v>
@@ -11512,7 +11464,7 @@
         <v>40</v>
       </c>
       <c r="AA87" t="s" s="2">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="AB87" s="2"/>
       <c r="AC87" t="s" s="2">
@@ -11554,7 +11506,7 @@
         <v>345</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C88" t="s" s="2">
         <v>40</v>
@@ -11576,7 +11528,7 @@
         <v>40</v>
       </c>
       <c r="J88" t="s" s="2">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="K88" t="s" s="2">
         <v>346</v>
@@ -11650,7 +11602,7 @@
         <v>40</v>
       </c>
       <c r="AJ88" t="s" s="2">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="AK88" t="s" s="2">
         <v>350</v>
@@ -11667,7 +11619,7 @@
         <v>345</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C89" t="s" s="2">
         <v>40</v>
@@ -11689,7 +11641,7 @@
         <v>40</v>
       </c>
       <c r="J89" t="s" s="2">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="K89" t="s" s="2">
         <v>346</v>
@@ -11712,7 +11664,7 @@
         <v>40</v>
       </c>
       <c r="S89" t="s" s="2">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="T89" t="s" s="2">
         <v>40</v>
@@ -11763,7 +11715,7 @@
         <v>40</v>
       </c>
       <c r="AJ89" t="s" s="2">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="AK89" t="s" s="2">
         <v>350</v>
@@ -11780,7 +11732,7 @@
         <v>345</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C90" t="s" s="2">
         <v>40</v>
@@ -11802,7 +11754,7 @@
         <v>40</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="K90" t="s" s="2">
         <v>346</v>
@@ -11825,7 +11777,7 @@
         <v>40</v>
       </c>
       <c r="S90" t="s" s="2">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="T90" t="s" s="2">
         <v>40</v>
@@ -11876,7 +11828,7 @@
         <v>40</v>
       </c>
       <c r="AJ90" t="s" s="2">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="AK90" t="s" s="2">
         <v>350</v>
@@ -11893,7 +11845,7 @@
         <v>345</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C91" t="s" s="2">
         <v>40</v>
@@ -11915,7 +11867,7 @@
         <v>40</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="K91" t="s" s="2">
         <v>346</v>
@@ -11938,7 +11890,7 @@
         <v>40</v>
       </c>
       <c r="S91" t="s" s="2">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="T91" t="s" s="2">
         <v>40</v>
@@ -11989,7 +11941,7 @@
         <v>40</v>
       </c>
       <c r="AJ91" t="s" s="2">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="AK91" t="s" s="2">
         <v>350</v>
@@ -12230,7 +12182,7 @@
         <v>298</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C94" t="s" s="2">
         <v>40</v>
@@ -12255,7 +12207,7 @@
         <v>200</v>
       </c>
       <c r="K94" t="s" s="2">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="L94" t="s" s="2">
         <v>301</v>
@@ -12324,7 +12276,7 @@
         <v>304</v>
       </c>
       <c r="AJ94" t="s" s="2">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="AK94" t="s" s="2">
         <v>305</v>
@@ -12667,7 +12619,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
         <v>310</v>
       </c>
@@ -12677,13 +12629,13 @@
       </c>
       <c r="D98" s="2"/>
       <c r="E98" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F98" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G98" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H98" t="s" s="2">
         <v>40</v>
@@ -12711,13 +12663,13 @@
       </c>
       <c r="P98" s="2"/>
       <c r="Q98" t="s" s="2">
-        <v>404</v>
+        <v>40</v>
       </c>
       <c r="R98" t="s" s="2">
         <v>40</v>
       </c>
       <c r="S98" t="s" s="2">
-        <v>404</v>
+        <v>40</v>
       </c>
       <c r="T98" t="s" s="2">
         <v>40</v>
@@ -12768,7 +12720,7 @@
         <v>40</v>
       </c>
       <c r="AJ98" t="s" s="2">
-        <v>405</v>
+        <v>40</v>
       </c>
       <c r="AK98" t="s" s="2">
         <v>190</v>
@@ -12827,10 +12779,10 @@
         <v>40</v>
       </c>
       <c r="R99" t="s" s="2">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="S99" t="s" s="2">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="T99" t="s" s="2">
         <v>40</v>
@@ -12881,7 +12833,7 @@
         <v>40</v>
       </c>
       <c r="AJ99" t="s" s="2">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="AK99" t="s" s="2">
         <v>135</v>
@@ -12893,7 +12845,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
         <v>323</v>
       </c>
@@ -12903,13 +12855,13 @@
       </c>
       <c r="D100" s="2"/>
       <c r="E100" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F100" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G100" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H100" t="s" s="2">
         <v>40</v>
@@ -12992,7 +12944,7 @@
         <v>40</v>
       </c>
       <c r="AJ100" t="s" s="2">
-        <v>387</v>
+        <v>40</v>
       </c>
       <c r="AK100" t="s" s="2">
         <v>328</v>
@@ -13255,7 +13207,7 @@
         <v>40</v>
       </c>
       <c r="J103" t="s" s="2">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="K103" t="s" s="2">
         <v>346</v>
@@ -13278,7 +13230,7 @@
         <v>40</v>
       </c>
       <c r="S103" t="s" s="2">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="T103" t="s" s="2">
         <v>40</v>
@@ -13329,7 +13281,7 @@
         <v>40</v>
       </c>
       <c r="AJ103" t="s" s="2">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="AK103" t="s" s="2">
         <v>350</v>
@@ -13343,7 +13295,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -13452,7 +13404,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -13522,10 +13474,10 @@
         <v>40</v>
       </c>
       <c r="AA105" t="s" s="2">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="AB105" t="s" s="2">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="AC105" t="s" s="2">
         <v>40</v>
@@ -13563,10 +13515,10 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B106" t="s" s="2">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C106" t="s" s="2">
         <v>40</v>
@@ -13588,13 +13540,13 @@
         <v>40</v>
       </c>
       <c r="J106" t="s" s="2">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
@@ -13674,7 +13626,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -13783,7 +13735,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -13853,10 +13805,10 @@
         <v>40</v>
       </c>
       <c r="AA108" t="s" s="2">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="AB108" t="s" s="2">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="AC108" t="s" s="2">
         <v>40</v>
@@ -13894,7 +13846,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -13920,13 +13872,13 @@
         <v>65</v>
       </c>
       <c r="K109" t="s" s="2">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="M109" t="s" s="2">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="N109" s="2"/>
       <c r="O109" t="s" s="2">
@@ -13934,7 +13886,7 @@
       </c>
       <c r="P109" s="2"/>
       <c r="Q109" t="s" s="2">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="R109" t="s" s="2">
         <v>40</v>
@@ -13976,7 +13928,7 @@
         <v>40</v>
       </c>
       <c r="AE109" t="s" s="2">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AF109" t="s" s="2">
         <v>52</v>
@@ -14005,7 +13957,7 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -14028,13 +13980,13 @@
         <v>40</v>
       </c>
       <c r="J110" t="s" s="2">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="K110" t="s" s="2">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="L110" t="s" s="2">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="M110" s="2"/>
       <c r="N110" s="2"/>
@@ -14085,7 +14037,7 @@
         <v>40</v>
       </c>
       <c r="AE110" t="s" s="2">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="AF110" t="s" s="2">
         <v>41</v>
@@ -14114,7 +14066,7 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -14140,13 +14092,13 @@
         <v>186</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="L111" t="s" s="2">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="M111" t="s" s="2">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="N111" s="2"/>
       <c r="O111" t="s" s="2">
@@ -14196,7 +14148,7 @@
         <v>40</v>
       </c>
       <c r="AE111" t="s" s="2">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="AF111" t="s" s="2">
         <v>41</v>
@@ -14205,7 +14157,7 @@
         <v>52</v>
       </c>
       <c r="AH111" t="s" s="2">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="AI111" t="s" s="2">
         <v>40</v>
@@ -14225,7 +14177,7 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -14251,13 +14203,13 @@
         <v>108</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="M112" t="s" s="2">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="N112" s="2"/>
       <c r="O112" t="s" s="2">
@@ -14307,7 +14259,7 @@
         <v>40</v>
       </c>
       <c r="AE112" t="s" s="2">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="AF112" t="s" s="2">
         <v>41</v>
@@ -14325,7 +14277,7 @@
         <v>40</v>
       </c>
       <c r="AK112" t="s" s="2">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="AL112" t="s" s="2">
         <v>40</v>
@@ -14336,7 +14288,7 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -14362,13 +14314,13 @@
         <v>186</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="M113" t="s" s="2">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="N113" s="2"/>
       <c r="O113" t="s" s="2">
@@ -14418,7 +14370,7 @@
         <v>40</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>41</v>
@@ -14674,7 +14626,7 @@
         <v>298</v>
       </c>
       <c r="B116" t="s" s="2">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="C116" t="s" s="2">
         <v>40</v>
@@ -14699,7 +14651,7 @@
         <v>200</v>
       </c>
       <c r="K116" t="s" s="2">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="L116" t="s" s="2">
         <v>301</v>
@@ -14768,7 +14720,7 @@
         <v>304</v>
       </c>
       <c r="AJ116" t="s" s="2">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="AK116" t="s" s="2">
         <v>305</v>
@@ -15111,7 +15063,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
         <v>310</v>
       </c>
@@ -15121,13 +15073,13 @@
       </c>
       <c r="D120" s="2"/>
       <c r="E120" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F120" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G120" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H120" t="s" s="2">
         <v>40</v>
@@ -15155,13 +15107,13 @@
       </c>
       <c r="P120" s="2"/>
       <c r="Q120" t="s" s="2">
-        <v>452</v>
+        <v>40</v>
       </c>
       <c r="R120" t="s" s="2">
         <v>40</v>
       </c>
       <c r="S120" t="s" s="2">
-        <v>452</v>
+        <v>40</v>
       </c>
       <c r="T120" t="s" s="2">
         <v>40</v>
@@ -15212,7 +15164,7 @@
         <v>40</v>
       </c>
       <c r="AJ120" t="s" s="2">
-        <v>453</v>
+        <v>40</v>
       </c>
       <c r="AK120" t="s" s="2">
         <v>190</v>
@@ -15271,10 +15223,10 @@
         <v>40</v>
       </c>
       <c r="R121" t="s" s="2">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="S121" t="s" s="2">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="T121" t="s" s="2">
         <v>40</v>
@@ -15325,7 +15277,7 @@
         <v>40</v>
       </c>
       <c r="AJ121" t="s" s="2">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="AK121" t="s" s="2">
         <v>135</v>
@@ -15436,7 +15388,7 @@
         <v>40</v>
       </c>
       <c r="AJ122" t="s" s="2">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="AK122" t="s" s="2">
         <v>328</v>
@@ -15699,7 +15651,7 @@
         <v>40</v>
       </c>
       <c r="J125" t="s" s="2">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="K125" t="s" s="2">
         <v>346</v>
@@ -15722,7 +15674,7 @@
         <v>40</v>
       </c>
       <c r="S125" t="s" s="2">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="T125" t="s" s="2">
         <v>40</v>
@@ -15773,7 +15725,7 @@
         <v>40</v>
       </c>
       <c r="AJ125" t="s" s="2">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="AK125" t="s" s="2">
         <v>350</v>
@@ -16014,7 +15966,7 @@
         <v>298</v>
       </c>
       <c r="B128" t="s" s="2">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="C128" t="s" s="2">
         <v>40</v>
@@ -16039,7 +15991,7 @@
         <v>200</v>
       </c>
       <c r="K128" t="s" s="2">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="L128" t="s" s="2">
         <v>301</v>
@@ -16108,7 +16060,7 @@
         <v>304</v>
       </c>
       <c r="AJ128" t="s" s="2">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="AK128" t="s" s="2">
         <v>305</v>
@@ -16451,7 +16403,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
         <v>310</v>
       </c>
@@ -16461,13 +16413,13 @@
       </c>
       <c r="D132" s="2"/>
       <c r="E132" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F132" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G132" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H132" t="s" s="2">
         <v>40</v>
@@ -16495,13 +16447,13 @@
       </c>
       <c r="P132" s="2"/>
       <c r="Q132" t="s" s="2">
-        <v>463</v>
+        <v>40</v>
       </c>
       <c r="R132" t="s" s="2">
         <v>40</v>
       </c>
       <c r="S132" t="s" s="2">
-        <v>463</v>
+        <v>40</v>
       </c>
       <c r="T132" t="s" s="2">
         <v>40</v>
@@ -16552,7 +16504,7 @@
         <v>40</v>
       </c>
       <c r="AJ132" t="s" s="2">
-        <v>464</v>
+        <v>40</v>
       </c>
       <c r="AK132" t="s" s="2">
         <v>190</v>
@@ -16611,10 +16563,10 @@
         <v>40</v>
       </c>
       <c r="R133" t="s" s="2">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="S133" t="s" s="2">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="T133" t="s" s="2">
         <v>40</v>
@@ -16665,7 +16617,7 @@
         <v>40</v>
       </c>
       <c r="AJ133" t="s" s="2">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="AK133" t="s" s="2">
         <v>135</v>
@@ -16677,7 +16629,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
         <v>323</v>
       </c>
@@ -16687,13 +16639,13 @@
       </c>
       <c r="D134" s="2"/>
       <c r="E134" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F134" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G134" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H134" t="s" s="2">
         <v>40</v>
@@ -16776,7 +16728,7 @@
         <v>40</v>
       </c>
       <c r="AJ134" t="s" s="2">
-        <v>467</v>
+        <v>40</v>
       </c>
       <c r="AK134" t="s" s="2">
         <v>328</v>
@@ -17086,7 +17038,7 @@
         <v>40</v>
       </c>
       <c r="AA137" t="s" s="2">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="AB137" s="2"/>
       <c r="AC137" t="s" s="2">
@@ -17128,7 +17080,7 @@
         <v>345</v>
       </c>
       <c r="B138" t="s" s="2">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="C138" t="s" s="2">
         <v>40</v>
@@ -17224,7 +17176,7 @@
         <v>40</v>
       </c>
       <c r="AJ138" t="s" s="2">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="AK138" t="s" s="2">
         <v>350</v>
@@ -17241,7 +17193,7 @@
         <v>345</v>
       </c>
       <c r="B139" t="s" s="2">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="C139" t="s" s="2">
         <v>40</v>
@@ -17263,7 +17215,7 @@
         <v>40</v>
       </c>
       <c r="J139" t="s" s="2">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="K139" t="s" s="2">
         <v>346</v>
@@ -17286,7 +17238,7 @@
         <v>40</v>
       </c>
       <c r="S139" t="s" s="2">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="T139" t="s" s="2">
         <v>40</v>
@@ -17337,7 +17289,7 @@
         <v>40</v>
       </c>
       <c r="AJ139" t="s" s="2">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="AK139" t="s" s="2">
         <v>350</v>
@@ -17351,7 +17303,7 @@
     </row>
     <row r="140" hidden="true">
       <c r="A140" t="s" s="2">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" t="s" s="2">
@@ -17460,7 +17412,7 @@
     </row>
     <row r="141" hidden="true">
       <c r="A141" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" t="s" s="2">
@@ -17530,10 +17482,10 @@
         <v>40</v>
       </c>
       <c r="AA141" t="s" s="2">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="AB141" t="s" s="2">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="AC141" t="s" s="2">
         <v>40</v>
@@ -17571,10 +17523,10 @@
     </row>
     <row r="142">
       <c r="A142" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B142" t="s" s="2">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="C142" t="s" s="2">
         <v>40</v>
@@ -17596,13 +17548,13 @@
         <v>40</v>
       </c>
       <c r="J142" t="s" s="2">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="K142" t="s" s="2">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="L142" t="s" s="2">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="M142" s="2"/>
       <c r="N142" s="2"/>
@@ -17682,7 +17634,7 @@
     </row>
     <row r="143" hidden="true">
       <c r="A143" t="s" s="2">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" t="s" s="2">
@@ -17791,7 +17743,7 @@
     </row>
     <row r="144" hidden="true">
       <c r="A144" t="s" s="2">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" t="s" s="2">
@@ -17861,10 +17813,10 @@
         <v>40</v>
       </c>
       <c r="AA144" t="s" s="2">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="AB144" t="s" s="2">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="AC144" t="s" s="2">
         <v>40</v>
@@ -17902,7 +17854,7 @@
     </row>
     <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
@@ -17928,13 +17880,13 @@
         <v>65</v>
       </c>
       <c r="K145" t="s" s="2">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="L145" t="s" s="2">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="M145" t="s" s="2">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="N145" s="2"/>
       <c r="O145" t="s" s="2">
@@ -17942,7 +17894,7 @@
       </c>
       <c r="P145" s="2"/>
       <c r="Q145" t="s" s="2">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="R145" t="s" s="2">
         <v>40</v>
@@ -17984,7 +17936,7 @@
         <v>40</v>
       </c>
       <c r="AE145" t="s" s="2">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AF145" t="s" s="2">
         <v>52</v>
@@ -18013,7 +17965,7 @@
     </row>
     <row r="146" hidden="true">
       <c r="A146" t="s" s="2">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" t="s" s="2">
@@ -18036,13 +17988,13 @@
         <v>40</v>
       </c>
       <c r="J146" t="s" s="2">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="K146" t="s" s="2">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="L146" t="s" s="2">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="M146" s="2"/>
       <c r="N146" s="2"/>
@@ -18093,7 +18045,7 @@
         <v>40</v>
       </c>
       <c r="AE146" t="s" s="2">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="AF146" t="s" s="2">
         <v>41</v>
@@ -18122,7 +18074,7 @@
     </row>
     <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" t="s" s="2">
@@ -18148,13 +18100,13 @@
         <v>186</v>
       </c>
       <c r="K147" t="s" s="2">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="L147" t="s" s="2">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="M147" t="s" s="2">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="N147" s="2"/>
       <c r="O147" t="s" s="2">
@@ -18204,7 +18156,7 @@
         <v>40</v>
       </c>
       <c r="AE147" t="s" s="2">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="AF147" t="s" s="2">
         <v>41</v>
@@ -18213,7 +18165,7 @@
         <v>52</v>
       </c>
       <c r="AH147" t="s" s="2">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="AI147" t="s" s="2">
         <v>40</v>
@@ -18233,7 +18185,7 @@
     </row>
     <row r="148" hidden="true">
       <c r="A148" t="s" s="2">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" t="s" s="2">
@@ -18259,13 +18211,13 @@
         <v>108</v>
       </c>
       <c r="K148" t="s" s="2">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="L148" t="s" s="2">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="M148" t="s" s="2">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="N148" s="2"/>
       <c r="O148" t="s" s="2">
@@ -18315,7 +18267,7 @@
         <v>40</v>
       </c>
       <c r="AE148" t="s" s="2">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="AF148" t="s" s="2">
         <v>41</v>
@@ -18333,7 +18285,7 @@
         <v>40</v>
       </c>
       <c r="AK148" t="s" s="2">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="AL148" t="s" s="2">
         <v>40</v>
@@ -18344,7 +18296,7 @@
     </row>
     <row r="149" hidden="true">
       <c r="A149" t="s" s="2">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" t="s" s="2">
@@ -18370,13 +18322,13 @@
         <v>186</v>
       </c>
       <c r="K149" t="s" s="2">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="L149" t="s" s="2">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="M149" t="s" s="2">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="N149" s="2"/>
       <c r="O149" t="s" s="2">
@@ -18426,7 +18378,7 @@
         <v>40</v>
       </c>
       <c r="AE149" t="s" s="2">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="AF149" t="s" s="2">
         <v>41</v>
@@ -18458,7 +18410,7 @@
         <v>345</v>
       </c>
       <c r="B150" t="s" s="2">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="C150" t="s" s="2">
         <v>40</v>
@@ -18480,7 +18432,7 @@
         <v>40</v>
       </c>
       <c r="J150" t="s" s="2">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="K150" t="s" s="2">
         <v>346</v>
@@ -18503,7 +18455,7 @@
         <v>40</v>
       </c>
       <c r="S150" t="s" s="2">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="T150" t="s" s="2">
         <v>40</v>
@@ -18554,7 +18506,7 @@
         <v>40</v>
       </c>
       <c r="AJ150" t="s" s="2">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="AK150" t="s" s="2">
         <v>350</v>
@@ -18568,7 +18520,7 @@
     </row>
     <row r="151" hidden="true">
       <c r="A151" t="s" s="2">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" t="s" s="2">
@@ -18677,7 +18629,7 @@
     </row>
     <row r="152" hidden="true">
       <c r="A152" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" t="s" s="2">
@@ -18747,10 +18699,10 @@
         <v>40</v>
       </c>
       <c r="AA152" t="s" s="2">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="AB152" t="s" s="2">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="AC152" t="s" s="2">
         <v>40</v>
@@ -18788,10 +18740,10 @@
     </row>
     <row r="153">
       <c r="A153" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B153" t="s" s="2">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="C153" t="s" s="2">
         <v>40</v>
@@ -18813,13 +18765,13 @@
         <v>40</v>
       </c>
       <c r="J153" t="s" s="2">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="K153" t="s" s="2">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="L153" t="s" s="2">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="M153" s="2"/>
       <c r="N153" s="2"/>
@@ -18899,7 +18851,7 @@
     </row>
     <row r="154" hidden="true">
       <c r="A154" t="s" s="2">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" t="s" s="2">
@@ -19008,7 +18960,7 @@
     </row>
     <row r="155" hidden="true">
       <c r="A155" t="s" s="2">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" t="s" s="2">
@@ -19078,10 +19030,10 @@
         <v>40</v>
       </c>
       <c r="AA155" t="s" s="2">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="AB155" t="s" s="2">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="AC155" t="s" s="2">
         <v>40</v>
@@ -19119,7 +19071,7 @@
     </row>
     <row r="156" hidden="true">
       <c r="A156" t="s" s="2">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" t="s" s="2">
@@ -19145,13 +19097,13 @@
         <v>65</v>
       </c>
       <c r="K156" t="s" s="2">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="L156" t="s" s="2">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="M156" t="s" s="2">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="N156" s="2"/>
       <c r="O156" t="s" s="2">
@@ -19159,7 +19111,7 @@
       </c>
       <c r="P156" s="2"/>
       <c r="Q156" t="s" s="2">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="R156" t="s" s="2">
         <v>40</v>
@@ -19201,7 +19153,7 @@
         <v>40</v>
       </c>
       <c r="AE156" t="s" s="2">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AF156" t="s" s="2">
         <v>52</v>
@@ -19230,7 +19182,7 @@
     </row>
     <row r="157" hidden="true">
       <c r="A157" t="s" s="2">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" t="s" s="2">
@@ -19253,13 +19205,13 @@
         <v>40</v>
       </c>
       <c r="J157" t="s" s="2">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="K157" t="s" s="2">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="L157" t="s" s="2">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="M157" s="2"/>
       <c r="N157" s="2"/>
@@ -19310,7 +19262,7 @@
         <v>40</v>
       </c>
       <c r="AE157" t="s" s="2">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="AF157" t="s" s="2">
         <v>41</v>
@@ -19339,7 +19291,7 @@
     </row>
     <row r="158" hidden="true">
       <c r="A158" t="s" s="2">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" t="s" s="2">
@@ -19365,13 +19317,13 @@
         <v>186</v>
       </c>
       <c r="K158" t="s" s="2">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="L158" t="s" s="2">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="M158" t="s" s="2">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="N158" s="2"/>
       <c r="O158" t="s" s="2">
@@ -19421,7 +19373,7 @@
         <v>40</v>
       </c>
       <c r="AE158" t="s" s="2">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="AF158" t="s" s="2">
         <v>41</v>
@@ -19430,7 +19382,7 @@
         <v>52</v>
       </c>
       <c r="AH158" t="s" s="2">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="AI158" t="s" s="2">
         <v>40</v>
@@ -19450,7 +19402,7 @@
     </row>
     <row r="159" hidden="true">
       <c r="A159" t="s" s="2">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" t="s" s="2">
@@ -19476,13 +19428,13 @@
         <v>108</v>
       </c>
       <c r="K159" t="s" s="2">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="L159" t="s" s="2">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="M159" t="s" s="2">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="N159" s="2"/>
       <c r="O159" t="s" s="2">
@@ -19532,7 +19484,7 @@
         <v>40</v>
       </c>
       <c r="AE159" t="s" s="2">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="AF159" t="s" s="2">
         <v>41</v>
@@ -19550,7 +19502,7 @@
         <v>40</v>
       </c>
       <c r="AK159" t="s" s="2">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="AL159" t="s" s="2">
         <v>40</v>
@@ -19561,7 +19513,7 @@
     </row>
     <row r="160" hidden="true">
       <c r="A160" t="s" s="2">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" t="s" s="2">
@@ -19587,13 +19539,13 @@
         <v>186</v>
       </c>
       <c r="K160" t="s" s="2">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="L160" t="s" s="2">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="M160" t="s" s="2">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="N160" s="2"/>
       <c r="O160" t="s" s="2">
@@ -19643,7 +19595,7 @@
         <v>40</v>
       </c>
       <c r="AE160" t="s" s="2">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="AF160" t="s" s="2">
         <v>41</v>
@@ -19899,7 +19851,7 @@
         <v>298</v>
       </c>
       <c r="B163" t="s" s="2">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="C163" t="s" s="2">
         <v>40</v>
@@ -19924,7 +19876,7 @@
         <v>200</v>
       </c>
       <c r="K163" t="s" s="2">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="L163" t="s" s="2">
         <v>301</v>
@@ -20336,7 +20288,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
         <v>310</v>
       </c>
@@ -20346,13 +20298,13 @@
       </c>
       <c r="D167" s="2"/>
       <c r="E167" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F167" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G167" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H167" t="s" s="2">
         <v>40</v>
@@ -20380,13 +20332,13 @@
       </c>
       <c r="P167" s="2"/>
       <c r="Q167" t="s" s="2">
-        <v>481</v>
+        <v>40</v>
       </c>
       <c r="R167" t="s" s="2">
         <v>40</v>
       </c>
       <c r="S167" t="s" s="2">
-        <v>463</v>
+        <v>40</v>
       </c>
       <c r="T167" t="s" s="2">
         <v>40</v>
@@ -20496,10 +20448,10 @@
         <v>40</v>
       </c>
       <c r="R168" t="s" s="2">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="S168" t="s" s="2">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="T168" t="s" s="2">
         <v>40</v>
@@ -20562,7 +20514,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
         <v>323</v>
       </c>
@@ -20572,13 +20524,13 @@
       </c>
       <c r="D169" s="2"/>
       <c r="E169" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F169" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G169" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H169" t="s" s="2">
         <v>40</v>
@@ -20924,7 +20876,7 @@
         <v>40</v>
       </c>
       <c r="J172" t="s" s="2">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="K172" t="s" s="2">
         <v>346</v>
@@ -20947,7 +20899,7 @@
         <v>40</v>
       </c>
       <c r="S172" t="s" s="2">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="T172" t="s" s="2">
         <v>40</v>
@@ -21012,7 +20964,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -21121,7 +21073,7 @@
     </row>
     <row r="174" hidden="true">
       <c r="A174" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
@@ -21191,10 +21143,10 @@
         <v>40</v>
       </c>
       <c r="AA174" t="s" s="2">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="AB174" t="s" s="2">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="AC174" t="s" s="2">
         <v>40</v>
@@ -21232,10 +21184,10 @@
     </row>
     <row r="175">
       <c r="A175" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B175" t="s" s="2">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="C175" t="s" s="2">
         <v>40</v>
@@ -21257,13 +21209,13 @@
         <v>40</v>
       </c>
       <c r="J175" t="s" s="2">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="K175" t="s" s="2">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="L175" t="s" s="2">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="M175" s="2"/>
       <c r="N175" s="2"/>
@@ -21343,7 +21295,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
@@ -21452,7 +21404,7 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
@@ -21522,10 +21474,10 @@
         <v>40</v>
       </c>
       <c r="AA177" t="s" s="2">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="AB177" t="s" s="2">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="AC177" t="s" s="2">
         <v>40</v>
@@ -21563,7 +21515,7 @@
     </row>
     <row r="178" hidden="true">
       <c r="A178" t="s" s="2">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -21589,13 +21541,13 @@
         <v>65</v>
       </c>
       <c r="K178" t="s" s="2">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="L178" t="s" s="2">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="M178" t="s" s="2">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="N178" s="2"/>
       <c r="O178" t="s" s="2">
@@ -21603,7 +21555,7 @@
       </c>
       <c r="P178" s="2"/>
       <c r="Q178" t="s" s="2">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="R178" t="s" s="2">
         <v>40</v>
@@ -21645,7 +21597,7 @@
         <v>40</v>
       </c>
       <c r="AE178" t="s" s="2">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AF178" t="s" s="2">
         <v>52</v>
@@ -21674,7 +21626,7 @@
     </row>
     <row r="179" hidden="true">
       <c r="A179" t="s" s="2">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -21697,13 +21649,13 @@
         <v>40</v>
       </c>
       <c r="J179" t="s" s="2">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="K179" t="s" s="2">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="L179" t="s" s="2">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="M179" s="2"/>
       <c r="N179" s="2"/>
@@ -21754,7 +21706,7 @@
         <v>40</v>
       </c>
       <c r="AE179" t="s" s="2">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="AF179" t="s" s="2">
         <v>41</v>
@@ -21783,7 +21735,7 @@
     </row>
     <row r="180" hidden="true">
       <c r="A180" t="s" s="2">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
@@ -21809,13 +21761,13 @@
         <v>186</v>
       </c>
       <c r="K180" t="s" s="2">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="L180" t="s" s="2">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="M180" t="s" s="2">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="N180" s="2"/>
       <c r="O180" t="s" s="2">
@@ -21865,7 +21817,7 @@
         <v>40</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>41</v>
@@ -21874,7 +21826,7 @@
         <v>52</v>
       </c>
       <c r="AH180" t="s" s="2">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="AI180" t="s" s="2">
         <v>40</v>
@@ -21894,7 +21846,7 @@
     </row>
     <row r="181" hidden="true">
       <c r="A181" t="s" s="2">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
@@ -21920,13 +21872,13 @@
         <v>108</v>
       </c>
       <c r="K181" t="s" s="2">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="L181" t="s" s="2">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="M181" t="s" s="2">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="N181" s="2"/>
       <c r="O181" t="s" s="2">
@@ -21976,7 +21928,7 @@
         <v>40</v>
       </c>
       <c r="AE181" t="s" s="2">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="AF181" t="s" s="2">
         <v>41</v>
@@ -21994,7 +21946,7 @@
         <v>40</v>
       </c>
       <c r="AK181" t="s" s="2">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="AL181" t="s" s="2">
         <v>40</v>
@@ -22005,7 +21957,7 @@
     </row>
     <row r="182" hidden="true">
       <c r="A182" t="s" s="2">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
@@ -22031,13 +21983,13 @@
         <v>186</v>
       </c>
       <c r="K182" t="s" s="2">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="L182" t="s" s="2">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="M182" t="s" s="2">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="N182" s="2"/>
       <c r="O182" t="s" s="2">
@@ -22087,7 +22039,7 @@
         <v>40</v>
       </c>
       <c r="AE182" t="s" s="2">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="AF182" t="s" s="2">
         <v>41</v>
@@ -22343,7 +22295,7 @@
         <v>298</v>
       </c>
       <c r="B185" t="s" s="2">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="C185" t="s" s="2">
         <v>40</v>
@@ -22368,7 +22320,7 @@
         <v>200</v>
       </c>
       <c r="K185" t="s" s="2">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="L185" t="s" s="2">
         <v>301</v>
@@ -22437,7 +22389,7 @@
         <v>304</v>
       </c>
       <c r="AJ185" t="s" s="2">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="AK185" t="s" s="2">
         <v>305</v>
@@ -22780,7 +22732,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
         <v>310</v>
       </c>
@@ -22790,13 +22742,13 @@
       </c>
       <c r="D189" s="2"/>
       <c r="E189" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F189" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G189" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H189" t="s" s="2">
         <v>40</v>
@@ -22824,13 +22776,13 @@
       </c>
       <c r="P189" s="2"/>
       <c r="Q189" t="s" s="2">
-        <v>489</v>
+        <v>40</v>
       </c>
       <c r="R189" t="s" s="2">
         <v>40</v>
       </c>
       <c r="S189" t="s" s="2">
-        <v>489</v>
+        <v>40</v>
       </c>
       <c r="T189" t="s" s="2">
         <v>40</v>
@@ -22881,7 +22833,7 @@
         <v>40</v>
       </c>
       <c r="AJ189" t="s" s="2">
-        <v>490</v>
+        <v>40</v>
       </c>
       <c r="AK189" t="s" s="2">
         <v>190</v>
@@ -22940,10 +22892,10 @@
         <v>40</v>
       </c>
       <c r="R190" t="s" s="2">
-        <v>491</v>
+        <v>476</v>
       </c>
       <c r="S190" t="s" s="2">
-        <v>491</v>
+        <v>476</v>
       </c>
       <c r="T190" t="s" s="2">
         <v>40</v>
@@ -22994,7 +22946,7 @@
         <v>40</v>
       </c>
       <c r="AJ190" t="s" s="2">
-        <v>492</v>
+        <v>477</v>
       </c>
       <c r="AK190" t="s" s="2">
         <v>135</v>
@@ -23006,7 +22958,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
         <v>323</v>
       </c>
@@ -23016,13 +22968,13 @@
       </c>
       <c r="D191" s="2"/>
       <c r="E191" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F191" t="s" s="2">
         <v>52</v>
       </c>
       <c r="G191" t="s" s="2">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H191" t="s" s="2">
         <v>40</v>
@@ -23105,7 +23057,7 @@
         <v>40</v>
       </c>
       <c r="AJ191" t="s" s="2">
-        <v>493</v>
+        <v>40</v>
       </c>
       <c r="AK191" t="s" s="2">
         <v>328</v>
@@ -23368,7 +23320,7 @@
         <v>40</v>
       </c>
       <c r="J194" t="s" s="2">
-        <v>494</v>
+        <v>478</v>
       </c>
       <c r="K194" t="s" s="2">
         <v>346</v>
@@ -23391,7 +23343,7 @@
         <v>40</v>
       </c>
       <c r="S194" t="s" s="2">
-        <v>495</v>
+        <v>479</v>
       </c>
       <c r="T194" t="s" s="2">
         <v>40</v>
@@ -23442,7 +23394,7 @@
         <v>40</v>
       </c>
       <c r="AJ194" t="s" s="2">
-        <v>496</v>
+        <v>480</v>
       </c>
       <c r="AK194" t="s" s="2">
         <v>350</v>

</xml_diff>